<commit_message>
Updated ~/raw from master
</commit_message>
<xml_diff>
--- a/raw/Raw and Age-Adjusted National Mortality Rates by Gender (2007 - 2020).xlsx
+++ b/raw/Raw and Age-Adjusted National Mortality Rates by Gender (2007 - 2020).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe353eac81e08534/Desktop/CJD_Epi-master/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernd/Desktop/CJD_Epi/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6467AB42-6CA1-439C-82FD-21C91C4EFA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DD166B-5F39-401A-A1C3-E8BC8E5194BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0495FF89-DCD0-B640-B32B-A7D1467293B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality Rates" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
   <si>
     <t>Notes</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
   <si>
     <t>---</t>
@@ -839,7 +842,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1127,7 +1130,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1135,31 +1138,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="43" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.19921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2007</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>2.7022299999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2007</v>
       </c>
@@ -1303,54 +1306,51 @@
         <v>2.6492399999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
       <c r="B4">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C4">
-        <v>2008</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
+        <v>2007</v>
       </c>
       <c r="F4">
-        <v>161</v>
+        <v>303</v>
       </c>
       <c r="G4">
-        <v>154604015</v>
+        <v>301231207</v>
       </c>
       <c r="H4">
-        <v>0.10414</v>
+        <v>0.10059</v>
       </c>
       <c r="I4">
-        <v>8.8050000000000003E-2</v>
+        <v>8.9260000000000006E-2</v>
       </c>
       <c r="J4">
-        <v>0.12021999999999999</v>
+        <v>0.11191</v>
       </c>
       <c r="K4">
-        <v>8.2100000000000003E-3</v>
+        <v>5.7800000000000004E-3</v>
       </c>
       <c r="L4">
-        <v>8.9469999999999994E-2</v>
+        <v>9.5259999999999997E-2</v>
       </c>
       <c r="M4">
-        <v>7.5139999999999998E-2</v>
+        <v>8.4220000000000003E-2</v>
       </c>
       <c r="N4">
-        <v>0.1038</v>
+        <v>0.10631</v>
       </c>
       <c r="O4">
-        <v>7.3099999999999997E-3</v>
+        <v>5.64E-3</v>
       </c>
       <c r="P4" s="1">
-        <v>2.8435200000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>5.3514699999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2008</v>
       </c>
@@ -1358,145 +1358,142 @@
         <v>2008</v>
       </c>
       <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>161</v>
+      </c>
+      <c r="G5">
+        <v>154604015</v>
+      </c>
+      <c r="H5">
+        <v>0.10414</v>
+      </c>
+      <c r="I5">
+        <v>8.8050000000000003E-2</v>
+      </c>
+      <c r="J5">
+        <v>0.12021999999999999</v>
+      </c>
+      <c r="K5">
+        <v>8.2100000000000003E-3</v>
+      </c>
+      <c r="L5">
+        <v>8.9469999999999994E-2</v>
+      </c>
+      <c r="M5">
+        <v>7.5139999999999998E-2</v>
+      </c>
+      <c r="N5">
+        <v>0.1038</v>
+      </c>
+      <c r="O5">
+        <v>7.3099999999999997E-3</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2.8435200000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2008</v>
+      </c>
+      <c r="C6">
+        <v>2008</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>168</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>149489951</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>0.11237999999999999</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>9.5390000000000003E-2</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <v>0.12938</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <v>8.6700000000000006E-3</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <v>0.12658</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <v>0.10711</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <v>0.14605000000000001</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <v>9.9299999999999996E-3</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P6" s="1">
         <v>2.96715E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>2008</v>
+      </c>
+      <c r="C7">
+        <v>2008</v>
+      </c>
+      <c r="F7">
+        <v>329</v>
+      </c>
+      <c r="G7">
+        <v>304093966</v>
+      </c>
+      <c r="H7">
+        <v>0.10818999999999999</v>
+      </c>
+      <c r="I7">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.11988</v>
+      </c>
+      <c r="K7">
+        <v>5.96E-3</v>
+      </c>
+      <c r="L7">
+        <v>0.10211000000000001</v>
+      </c>
+      <c r="M7">
+        <v>9.0660000000000004E-2</v>
+      </c>
+      <c r="N7">
+        <v>0.11355999999999999</v>
+      </c>
+      <c r="O7">
+        <v>5.8399999999999997E-3</v>
+      </c>
+      <c r="P7" s="1">
+        <v>5.8106699999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B8">
         <v>2009</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>2009</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>164</v>
-      </c>
-      <c r="G6">
-        <v>155964075</v>
-      </c>
-      <c r="H6">
-        <v>0.10514999999999999</v>
-      </c>
-      <c r="I6">
-        <v>8.906E-2</v>
-      </c>
-      <c r="J6">
-        <v>0.12125</v>
-      </c>
-      <c r="K6">
-        <v>8.2100000000000003E-3</v>
-      </c>
-      <c r="L6">
-        <v>8.9469999999999994E-2</v>
-      </c>
-      <c r="M6">
-        <v>7.5310000000000002E-2</v>
-      </c>
-      <c r="N6">
-        <v>0.10364</v>
-      </c>
-      <c r="O6">
-        <v>7.2300000000000003E-3</v>
-      </c>
-      <c r="P6" s="1">
-        <v>2.8965000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>2009</v>
-      </c>
-      <c r="C7">
-        <v>2009</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>158</v>
-      </c>
-      <c r="G7">
-        <v>150807454</v>
-      </c>
-      <c r="H7">
-        <v>0.10477</v>
-      </c>
-      <c r="I7">
-        <v>8.8429999999999995E-2</v>
-      </c>
-      <c r="J7">
-        <v>0.12111</v>
-      </c>
-      <c r="K7">
-        <v>8.3400000000000002E-3</v>
-      </c>
-      <c r="L7">
-        <v>9.9010000000000001E-2</v>
-      </c>
-      <c r="M7">
-        <v>8.2960000000000006E-2</v>
-      </c>
-      <c r="N7">
-        <v>0.11506</v>
-      </c>
-      <c r="O7">
-        <v>8.1899999999999994E-3</v>
-      </c>
-      <c r="P7" s="1">
-        <v>2.7905300000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>2010</v>
-      </c>
-      <c r="C8">
-        <v>2010</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1505,45 +1502,45 @@
         <v>17</v>
       </c>
       <c r="F8">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G8">
-        <v>156964212</v>
+        <v>155964075</v>
       </c>
       <c r="H8">
-        <v>0.12041</v>
+        <v>0.10514999999999999</v>
       </c>
       <c r="I8">
-        <v>0.10324</v>
+        <v>8.906E-2</v>
       </c>
       <c r="J8">
-        <v>0.13758000000000001</v>
+        <v>0.12125</v>
       </c>
       <c r="K8">
-        <v>8.7600000000000004E-3</v>
+        <v>8.2100000000000003E-3</v>
       </c>
       <c r="L8">
-        <v>9.3710000000000002E-2</v>
+        <v>8.9469999999999994E-2</v>
       </c>
       <c r="M8">
-        <v>8.0240000000000006E-2</v>
+        <v>7.5310000000000002E-2</v>
       </c>
       <c r="N8">
-        <v>0.10718</v>
+        <v>0.10364</v>
       </c>
       <c r="O8">
-        <v>6.8700000000000002E-3</v>
+        <v>7.2300000000000003E-3</v>
       </c>
       <c r="P8" s="1">
-        <v>3.3380399999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2.8965000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="C9">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -1552,233 +1549,227 @@
         <v>19</v>
       </c>
       <c r="F9">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G9">
-        <v>151781326</v>
+        <v>150807454</v>
       </c>
       <c r="H9">
-        <v>0.11003</v>
+        <v>0.10477</v>
       </c>
       <c r="I9">
-        <v>9.3340000000000006E-2</v>
+        <v>8.8429999999999995E-2</v>
       </c>
       <c r="J9">
-        <v>0.12670999999999999</v>
+        <v>0.12111</v>
       </c>
       <c r="K9">
-        <v>8.5100000000000002E-3</v>
+        <v>8.3400000000000002E-3</v>
       </c>
       <c r="L9">
-        <v>0.10578</v>
+        <v>9.9010000000000001E-2</v>
       </c>
       <c r="M9">
-        <v>8.9039999999999994E-2</v>
+        <v>8.2960000000000006E-2</v>
       </c>
       <c r="N9">
-        <v>0.12253</v>
+        <v>0.11506</v>
       </c>
       <c r="O9">
-        <v>8.5400000000000007E-3</v>
+        <v>8.1899999999999994E-3</v>
       </c>
       <c r="P9" s="1">
-        <v>2.9494900000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2.7905300000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
       <c r="B10">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C10">
-        <v>2011</v>
-      </c>
-      <c r="D10" t="s">
+        <v>2009</v>
+      </c>
+      <c r="F10">
+        <v>322</v>
+      </c>
+      <c r="G10">
+        <v>306771529</v>
+      </c>
+      <c r="H10">
+        <v>0.10496</v>
+      </c>
+      <c r="I10">
+        <v>9.35E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.11643000000000001</v>
+      </c>
+      <c r="K10">
+        <v>5.8500000000000002E-3</v>
+      </c>
+      <c r="L10">
+        <v>8.9469999999999994E-2</v>
+      </c>
+      <c r="M10">
+        <v>7.9409999999999994E-2</v>
+      </c>
+      <c r="N10">
+        <v>9.9540000000000003E-2</v>
+      </c>
+      <c r="O10">
+        <v>5.1399999999999996E-3</v>
+      </c>
+      <c r="P10" s="1">
+        <v>5.6870400000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>2010</v>
+      </c>
+      <c r="C11">
+        <v>2010</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>17</v>
-      </c>
-      <c r="F10">
-        <v>194</v>
-      </c>
-      <c r="G10">
-        <v>158301098</v>
-      </c>
-      <c r="H10">
-        <v>0.12255000000000001</v>
-      </c>
-      <c r="I10">
-        <v>0.10531</v>
-      </c>
-      <c r="J10">
-        <v>0.13980000000000001</v>
-      </c>
-      <c r="K10">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="L10">
-        <v>9.8769999999999997E-2</v>
-      </c>
-      <c r="M10">
-        <v>8.4430000000000005E-2</v>
-      </c>
-      <c r="N10">
-        <v>0.11311</v>
-      </c>
-      <c r="O10">
-        <v>7.3200000000000001E-3</v>
-      </c>
-      <c r="P10" s="1">
-        <v>3.4263500000000002E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>2011</v>
-      </c>
-      <c r="C11">
-        <v>2011</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
       </c>
       <c r="F11">
         <v>189</v>
       </c>
       <c r="G11">
-        <v>153290819</v>
+        <v>156964212</v>
       </c>
       <c r="H11">
-        <v>0.12330000000000001</v>
+        <v>0.12041</v>
       </c>
       <c r="I11">
-        <v>0.10571999999999999</v>
+        <v>0.10324</v>
       </c>
       <c r="J11">
-        <v>0.14087</v>
+        <v>0.13758000000000001</v>
       </c>
       <c r="K11">
-        <v>8.9700000000000005E-3</v>
+        <v>8.7600000000000004E-3</v>
       </c>
       <c r="L11">
-        <v>0.11663</v>
+        <v>9.3710000000000002E-2</v>
       </c>
       <c r="M11">
-        <v>9.9409999999999998E-2</v>
+        <v>8.0240000000000006E-2</v>
       </c>
       <c r="N11">
-        <v>0.13383999999999999</v>
+        <v>0.10718</v>
       </c>
       <c r="O11">
-        <v>8.7799999999999996E-3</v>
+        <v>6.8700000000000002E-3</v>
       </c>
       <c r="P11" s="1">
         <v>3.3380399999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C12">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F12">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="G12">
-        <v>159421973</v>
+        <v>151781326</v>
       </c>
       <c r="H12">
-        <v>0.11354</v>
+        <v>0.11003</v>
       </c>
       <c r="I12">
-        <v>9.6990000000000007E-2</v>
+        <v>9.3340000000000006E-2</v>
       </c>
       <c r="J12">
-        <v>0.13008</v>
+        <v>0.12670999999999999</v>
       </c>
       <c r="K12">
-        <v>8.4399999999999996E-3</v>
+        <v>8.5100000000000002E-3</v>
       </c>
       <c r="L12">
-        <v>9.2160000000000006E-2</v>
+        <v>0.10578</v>
       </c>
       <c r="M12">
-        <v>7.8390000000000001E-2</v>
+        <v>8.9039999999999994E-2</v>
       </c>
       <c r="N12">
-        <v>0.10593</v>
+        <v>0.12253</v>
       </c>
       <c r="O12">
-        <v>7.0299999999999998E-3</v>
+        <v>8.5400000000000007E-3</v>
       </c>
       <c r="P12" s="1">
-        <v>3.1967500000000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2.9494900000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
       <c r="B13">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C13">
-        <v>2012</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
+        <v>2010</v>
       </c>
       <c r="F13">
-        <v>157</v>
+        <v>356</v>
       </c>
       <c r="G13">
-        <v>154492067</v>
+        <v>308745538</v>
       </c>
       <c r="H13">
-        <v>0.10162</v>
+        <v>0.11531</v>
       </c>
       <c r="I13">
-        <v>8.5730000000000001E-2</v>
+        <v>0.10333000000000001</v>
       </c>
       <c r="J13">
-        <v>0.11752</v>
+        <v>0.12728</v>
       </c>
       <c r="K13">
-        <v>8.1099999999999992E-3</v>
+        <v>6.11E-3</v>
       </c>
       <c r="L13">
-        <v>9.1319999999999998E-2</v>
+        <v>9.9750000000000005E-2</v>
       </c>
       <c r="M13">
-        <v>7.6249999999999998E-2</v>
+        <v>8.9209999999999998E-2</v>
       </c>
       <c r="N13">
-        <v>0.10638</v>
+        <v>0.11029</v>
       </c>
       <c r="O13">
-        <v>7.6899999999999998E-3</v>
+        <v>5.3800000000000002E-3</v>
       </c>
       <c r="P13" s="1">
-        <v>2.7728699999999998E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.2875299999999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C14">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1787,45 +1778,45 @@
         <v>17</v>
       </c>
       <c r="F14">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="G14">
-        <v>160477237</v>
+        <v>158301098</v>
       </c>
       <c r="H14">
-        <v>0.13647000000000001</v>
+        <v>0.12255000000000001</v>
       </c>
       <c r="I14">
-        <v>0.11839</v>
+        <v>0.10531</v>
       </c>
       <c r="J14">
-        <v>0.15454000000000001</v>
+        <v>0.13980000000000001</v>
       </c>
       <c r="K14">
-        <v>9.2200000000000008E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="L14">
-        <v>0.10324999999999999</v>
+        <v>9.8769999999999997E-2</v>
       </c>
       <c r="M14">
-        <v>8.9130000000000001E-2</v>
+        <v>8.4430000000000005E-2</v>
       </c>
       <c r="N14">
-        <v>0.11737</v>
+        <v>0.11311</v>
       </c>
       <c r="O14">
-        <v>7.1999999999999998E-3</v>
+        <v>7.3200000000000001E-3</v>
       </c>
       <c r="P14" s="1">
-        <v>3.8678900000000002E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>3.4263500000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C15">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
@@ -1834,233 +1825,227 @@
         <v>19</v>
       </c>
       <c r="F15">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="G15">
-        <v>155651602</v>
+        <v>153290819</v>
       </c>
       <c r="H15">
-        <v>0.13427</v>
+        <v>0.12330000000000001</v>
       </c>
       <c r="I15">
-        <v>0.11607000000000001</v>
+        <v>0.10571999999999999</v>
       </c>
       <c r="J15">
-        <v>0.15248</v>
+        <v>0.14087</v>
       </c>
       <c r="K15">
-        <v>9.2899999999999996E-3</v>
+        <v>8.9700000000000005E-3</v>
       </c>
       <c r="L15">
-        <v>0.11279</v>
+        <v>0.11663</v>
       </c>
       <c r="M15">
-        <v>9.6780000000000005E-2</v>
+        <v>9.9409999999999998E-2</v>
       </c>
       <c r="N15">
-        <v>0.12878999999999999</v>
+        <v>0.13383999999999999</v>
       </c>
       <c r="O15">
-        <v>8.1700000000000002E-3</v>
+        <v>8.7799999999999996E-3</v>
       </c>
       <c r="P15" s="1">
-        <v>3.6912800000000003E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>3.3380399999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
       <c r="B16">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C16">
-        <v>2014</v>
-      </c>
-      <c r="D16" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F16">
+        <v>383</v>
+      </c>
+      <c r="G16">
+        <v>311591917</v>
+      </c>
+      <c r="H16">
+        <v>0.12292</v>
+      </c>
+      <c r="I16">
+        <v>0.11061</v>
+      </c>
+      <c r="J16">
+        <v>0.13522999999999999</v>
+      </c>
+      <c r="K16">
+        <v>6.28E-3</v>
+      </c>
+      <c r="L16">
+        <v>0.10692</v>
+      </c>
+      <c r="M16">
+        <v>9.5890000000000003E-2</v>
+      </c>
+      <c r="N16">
+        <v>0.11795</v>
+      </c>
+      <c r="O16">
+        <v>5.6299999999999996E-3</v>
+      </c>
+      <c r="P16" s="1">
+        <v>6.7643900000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>2012</v>
+      </c>
+      <c r="C17">
+        <v>2012</v>
+      </c>
+      <c r="D17" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="F16">
-        <v>202</v>
-      </c>
-      <c r="G16">
-        <v>161920569</v>
-      </c>
-      <c r="H16">
-        <v>0.12475</v>
-      </c>
-      <c r="I16">
-        <v>0.10755000000000001</v>
-      </c>
-      <c r="J16">
-        <v>0.14196</v>
-      </c>
-      <c r="K16">
-        <v>8.7799999999999996E-3</v>
-      </c>
-      <c r="L16">
-        <v>8.8660000000000003E-2</v>
-      </c>
-      <c r="M16">
-        <v>7.603E-2</v>
-      </c>
-      <c r="N16">
-        <v>0.10129000000000001</v>
-      </c>
-      <c r="O16">
-        <v>6.45E-3</v>
-      </c>
-      <c r="P16" s="1">
-        <v>3.5676399999999997E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>2014</v>
-      </c>
-      <c r="C17">
-        <v>2014</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="F17">
+        <v>181</v>
+      </c>
+      <c r="G17">
+        <v>159421973</v>
+      </c>
+      <c r="H17">
+        <v>0.11354</v>
+      </c>
+      <c r="I17">
+        <v>9.6990000000000007E-2</v>
+      </c>
+      <c r="J17">
+        <v>0.13008</v>
+      </c>
+      <c r="K17">
+        <v>8.4399999999999996E-3</v>
+      </c>
+      <c r="L17">
+        <v>9.2160000000000006E-2</v>
+      </c>
+      <c r="M17">
+        <v>7.8390000000000001E-2</v>
+      </c>
+      <c r="N17">
+        <v>0.10593</v>
+      </c>
+      <c r="O17">
+        <v>7.0299999999999998E-3</v>
+      </c>
+      <c r="P17" s="1">
+        <v>3.1967500000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>2012</v>
+      </c>
+      <c r="C18">
+        <v>2012</v>
+      </c>
+      <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="F17">
-        <v>200</v>
-      </c>
-      <c r="G17">
-        <v>156936487</v>
-      </c>
-      <c r="H17">
-        <v>0.12744</v>
-      </c>
-      <c r="I17">
-        <v>0.10978</v>
-      </c>
-      <c r="J17">
-        <v>0.14510000000000001</v>
-      </c>
-      <c r="K17">
-        <v>9.0100000000000006E-3</v>
-      </c>
-      <c r="L17">
-        <v>0.11589000000000001</v>
-      </c>
-      <c r="M17">
-        <v>9.9529999999999993E-2</v>
-      </c>
-      <c r="N17">
-        <v>0.13225000000000001</v>
-      </c>
-      <c r="O17">
-        <v>8.3499999999999998E-3</v>
-      </c>
-      <c r="P17" s="1">
-        <v>3.5323199999999999E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>2015</v>
-      </c>
-      <c r="C18">
-        <v>2015</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
       <c r="F18">
-        <v>227</v>
+        <v>157</v>
       </c>
       <c r="G18">
-        <v>163189523</v>
+        <v>154492067</v>
       </c>
       <c r="H18">
-        <v>0.1391</v>
+        <v>0.10162</v>
       </c>
       <c r="I18">
-        <v>0.12101000000000001</v>
+        <v>8.5730000000000001E-2</v>
       </c>
       <c r="J18">
-        <v>0.15720000000000001</v>
+        <v>0.11752</v>
       </c>
       <c r="K18">
-        <v>9.2300000000000004E-3</v>
+        <v>8.1099999999999992E-3</v>
       </c>
       <c r="L18">
-        <v>0.1114</v>
+        <v>9.1319999999999998E-2</v>
       </c>
       <c r="M18">
-        <v>9.6149999999999999E-2</v>
+        <v>7.6249999999999998E-2</v>
       </c>
       <c r="N18">
-        <v>0.12665999999999999</v>
+        <v>0.10638</v>
       </c>
       <c r="O18">
-        <v>7.7799999999999996E-3</v>
+        <v>7.6899999999999998E-3</v>
       </c>
       <c r="P18" s="1">
-        <v>4.0091799999999997E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+        <v>2.7728699999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
       <c r="B19">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="C19">
-        <v>2015</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>19</v>
+        <v>2012</v>
       </c>
       <c r="F19">
-        <v>223</v>
+        <v>338</v>
       </c>
       <c r="G19">
-        <v>158229297</v>
+        <v>313914040</v>
       </c>
       <c r="H19">
-        <v>0.14093</v>
+        <v>0.10767</v>
       </c>
       <c r="I19">
-        <v>0.12243999999999999</v>
+        <v>9.6189999999999998E-2</v>
       </c>
       <c r="J19">
-        <v>0.15942999999999999</v>
+        <v>0.11915000000000001</v>
       </c>
       <c r="K19">
-        <v>9.4400000000000005E-3</v>
+        <v>5.8599999999999998E-3</v>
       </c>
       <c r="L19">
-        <v>0.11589000000000001</v>
+        <v>9.2160000000000006E-2</v>
       </c>
       <c r="M19">
-        <v>0.10014000000000001</v>
+        <v>8.1970000000000001E-2</v>
       </c>
       <c r="N19">
-        <v>0.13164000000000001</v>
+        <v>0.10235</v>
       </c>
       <c r="O19">
-        <v>8.0400000000000003E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="P19" s="1">
-        <v>3.9385400000000001E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+        <v>5.9696199999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="C20">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -2069,45 +2054,45 @@
         <v>17</v>
       </c>
       <c r="F20">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="G20">
-        <v>164048590</v>
+        <v>160477237</v>
       </c>
       <c r="H20">
-        <v>0.13897999999999999</v>
+        <v>0.13647000000000001</v>
       </c>
       <c r="I20">
-        <v>0.12094000000000001</v>
+        <v>0.11839</v>
       </c>
       <c r="J20">
-        <v>0.15701999999999999</v>
+        <v>0.15454000000000001</v>
       </c>
       <c r="K20">
-        <v>9.1999999999999998E-3</v>
+        <v>9.2200000000000008E-3</v>
       </c>
       <c r="L20">
-        <v>0.1048</v>
+        <v>0.10324999999999999</v>
       </c>
       <c r="M20">
-        <v>9.1079999999999994E-2</v>
+        <v>8.9130000000000001E-2</v>
       </c>
       <c r="N20">
-        <v>0.11852</v>
+        <v>0.11737</v>
       </c>
       <c r="O20">
-        <v>7.0000000000000001E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="P20" s="1">
-        <v>4.0268499999999999E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+        <v>3.8678900000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="C21">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -2116,233 +2101,227 @@
         <v>19</v>
       </c>
       <c r="F21">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="G21">
-        <v>159078923</v>
+        <v>155651602</v>
       </c>
       <c r="H21">
-        <v>0.14521000000000001</v>
+        <v>0.13427</v>
       </c>
       <c r="I21">
-        <v>0.12648000000000001</v>
+        <v>0.11607000000000001</v>
       </c>
       <c r="J21">
-        <v>0.16394</v>
+        <v>0.15248</v>
       </c>
       <c r="K21">
-        <v>9.5499999999999995E-3</v>
+        <v>9.2899999999999996E-3</v>
       </c>
       <c r="L21">
-        <v>0.12772</v>
+        <v>0.11279</v>
       </c>
       <c r="M21">
-        <v>0.11076</v>
+        <v>9.6780000000000005E-2</v>
       </c>
       <c r="N21">
-        <v>0.14466999999999999</v>
+        <v>0.12878999999999999</v>
       </c>
       <c r="O21">
-        <v>8.6499999999999997E-3</v>
+        <v>8.1700000000000002E-3</v>
       </c>
       <c r="P21" s="1">
-        <v>4.0798300000000003E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+        <v>3.6912800000000003E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
       <c r="B22">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C22">
-        <v>2017</v>
-      </c>
-      <c r="D22" t="s">
+        <v>2013</v>
+      </c>
+      <c r="F22">
+        <v>428</v>
+      </c>
+      <c r="G22">
+        <v>316128839</v>
+      </c>
+      <c r="H22">
+        <v>0.13539000000000001</v>
+      </c>
+      <c r="I22">
+        <v>0.12256</v>
+      </c>
+      <c r="J22">
+        <v>0.14821000000000001</v>
+      </c>
+      <c r="K22">
+        <v>6.5399999999999998E-3</v>
+      </c>
+      <c r="L22">
+        <v>0.10618</v>
+      </c>
+      <c r="M22">
+        <v>9.5659999999999995E-2</v>
+      </c>
+      <c r="N22">
+        <v>0.11670999999999999</v>
+      </c>
+      <c r="O22">
+        <v>5.3699999999999998E-3</v>
+      </c>
+      <c r="P22" s="1">
+        <v>7.5591699999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>2014</v>
+      </c>
+      <c r="C23">
+        <v>2014</v>
+      </c>
+      <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>17</v>
       </c>
-      <c r="F22">
-        <v>242</v>
-      </c>
-      <c r="G22">
-        <v>165311059</v>
-      </c>
-      <c r="H22">
-        <v>0.14638999999999999</v>
-      </c>
-      <c r="I22">
-        <v>0.12795000000000001</v>
-      </c>
-      <c r="J22">
-        <v>0.16483</v>
-      </c>
-      <c r="K22">
-        <v>9.41E-3</v>
-      </c>
-      <c r="L22">
-        <v>0.10773000000000001</v>
-      </c>
-      <c r="M22">
-        <v>9.3670000000000003E-2</v>
-      </c>
-      <c r="N22">
-        <v>0.12180000000000001</v>
-      </c>
-      <c r="O22">
-        <v>7.1799999999999998E-3</v>
-      </c>
-      <c r="P22" s="1">
-        <v>4.2741099999999997E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>2017</v>
-      </c>
-      <c r="C23">
-        <v>2017</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="F23">
+        <v>202</v>
+      </c>
+      <c r="G23">
+        <v>161920569</v>
+      </c>
+      <c r="H23">
+        <v>0.12475</v>
+      </c>
+      <c r="I23">
+        <v>0.10755000000000001</v>
+      </c>
+      <c r="J23">
+        <v>0.14196</v>
+      </c>
+      <c r="K23">
+        <v>8.7799999999999996E-3</v>
+      </c>
+      <c r="L23">
+        <v>8.8660000000000003E-2</v>
+      </c>
+      <c r="M23">
+        <v>7.603E-2</v>
+      </c>
+      <c r="N23">
+        <v>0.10129000000000001</v>
+      </c>
+      <c r="O23">
+        <v>6.45E-3</v>
+      </c>
+      <c r="P23" s="1">
+        <v>3.5676399999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>2014</v>
+      </c>
+      <c r="C24">
+        <v>2014</v>
+      </c>
+      <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>19</v>
       </c>
-      <c r="F23">
-        <v>216</v>
-      </c>
-      <c r="G23">
-        <v>160408119</v>
-      </c>
-      <c r="H23">
-        <v>0.13466</v>
-      </c>
-      <c r="I23">
-        <v>0.1167</v>
-      </c>
-      <c r="J23">
-        <v>0.15261</v>
-      </c>
-      <c r="K23">
-        <v>9.1599999999999997E-3</v>
-      </c>
-      <c r="L23">
-        <v>0.11817999999999999</v>
-      </c>
-      <c r="M23">
-        <v>0.10181999999999999</v>
-      </c>
-      <c r="N23">
-        <v>0.13453999999999999</v>
-      </c>
-      <c r="O23">
+      <c r="F24">
+        <v>200</v>
+      </c>
+      <c r="G24">
+        <v>156936487</v>
+      </c>
+      <c r="H24">
+        <v>0.12744</v>
+      </c>
+      <c r="I24">
+        <v>0.10978</v>
+      </c>
+      <c r="J24">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="K24">
+        <v>9.0100000000000006E-3</v>
+      </c>
+      <c r="L24">
+        <v>0.11589000000000001</v>
+      </c>
+      <c r="M24">
+        <v>9.9529999999999993E-2</v>
+      </c>
+      <c r="N24">
+        <v>0.13225000000000001</v>
+      </c>
+      <c r="O24">
         <v>8.3499999999999998E-3</v>
       </c>
-      <c r="P23" s="1">
-        <v>3.8149099999999998E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>2018</v>
-      </c>
-      <c r="C24">
-        <v>2018</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24">
-        <v>227</v>
-      </c>
-      <c r="G24">
-        <v>166038755</v>
-      </c>
-      <c r="H24">
-        <v>0.13672000000000001</v>
-      </c>
-      <c r="I24">
-        <v>0.11892999999999999</v>
-      </c>
-      <c r="J24">
-        <v>0.1545</v>
-      </c>
-      <c r="K24">
-        <v>9.0699999999999999E-3</v>
-      </c>
-      <c r="L24">
-        <v>9.8199999999999996E-2</v>
-      </c>
-      <c r="M24">
-        <v>8.4919999999999995E-2</v>
-      </c>
-      <c r="N24">
-        <v>0.11147</v>
-      </c>
-      <c r="O24">
-        <v>6.77E-3</v>
-      </c>
       <c r="P24" s="1">
-        <v>4.0091799999999997E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+        <v>3.5323199999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
       <c r="B25">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C25">
-        <v>2018</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
-        <v>19</v>
+        <v>2014</v>
       </c>
       <c r="F25">
-        <v>213</v>
+        <v>402</v>
       </c>
       <c r="G25">
-        <v>161128679</v>
+        <v>318857056</v>
       </c>
       <c r="H25">
-        <v>0.13219</v>
+        <v>0.12608</v>
       </c>
       <c r="I25">
-        <v>0.11444</v>
+        <v>0.11375</v>
       </c>
       <c r="J25">
-        <v>0.14995</v>
+        <v>0.1384</v>
       </c>
       <c r="K25">
-        <v>9.0600000000000003E-3</v>
+        <v>6.2899999999999996E-3</v>
       </c>
       <c r="L25">
-        <v>0.11296</v>
+        <v>0.10635</v>
       </c>
       <c r="M25">
-        <v>9.6949999999999995E-2</v>
+        <v>9.572E-2</v>
       </c>
       <c r="N25">
-        <v>0.12897</v>
+        <v>0.11698</v>
       </c>
       <c r="O25">
-        <v>8.1700000000000002E-3</v>
+        <v>5.4200000000000003E-3</v>
       </c>
       <c r="P25" s="1">
-        <v>3.7619199999999998E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+        <v>7.0999599999999996E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C26">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -2351,45 +2330,45 @@
         <v>17</v>
       </c>
       <c r="F26">
-        <v>259</v>
+        <v>227</v>
       </c>
       <c r="G26">
-        <v>166582199</v>
+        <v>163189523</v>
       </c>
       <c r="H26">
-        <v>0.15548000000000001</v>
+        <v>0.1391</v>
       </c>
       <c r="I26">
-        <v>0.13653999999999999</v>
+        <v>0.12101000000000001</v>
       </c>
       <c r="J26">
-        <v>0.17441000000000001</v>
+        <v>0.15720000000000001</v>
       </c>
       <c r="K26">
-        <v>9.6600000000000002E-3</v>
+        <v>9.2300000000000004E-3</v>
       </c>
       <c r="L26">
-        <v>0.10985</v>
+        <v>0.1114</v>
       </c>
       <c r="M26">
-        <v>9.6259999999999998E-2</v>
+        <v>9.6149999999999999E-2</v>
       </c>
       <c r="N26">
-        <v>0.12345</v>
+        <v>0.12665999999999999</v>
       </c>
       <c r="O26">
-        <v>6.9300000000000004E-3</v>
+        <v>7.7799999999999996E-3</v>
       </c>
       <c r="P26" s="1">
-        <v>4.5743600000000002E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+        <v>4.0091799999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C27">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -2398,131 +2377,809 @@
         <v>19</v>
       </c>
       <c r="F27">
+        <v>223</v>
+      </c>
+      <c r="G27">
+        <v>158229297</v>
+      </c>
+      <c r="H27">
+        <v>0.14093</v>
+      </c>
+      <c r="I27">
+        <v>0.12243999999999999</v>
+      </c>
+      <c r="J27">
+        <v>0.15942999999999999</v>
+      </c>
+      <c r="K27">
+        <v>9.4400000000000005E-3</v>
+      </c>
+      <c r="L27">
+        <v>0.11589000000000001</v>
+      </c>
+      <c r="M27">
+        <v>0.10014000000000001</v>
+      </c>
+      <c r="N27">
+        <v>0.13164000000000001</v>
+      </c>
+      <c r="O27">
+        <v>8.0400000000000003E-3</v>
+      </c>
+      <c r="P27" s="1">
+        <v>3.9385400000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>2015</v>
+      </c>
+      <c r="C28">
+        <v>2015</v>
+      </c>
+      <c r="F28">
+        <v>450</v>
+      </c>
+      <c r="G28">
+        <v>321418820</v>
+      </c>
+      <c r="H28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I28">
+        <v>0.12706999999999999</v>
+      </c>
+      <c r="J28">
+        <v>0.15293999999999999</v>
+      </c>
+      <c r="K28">
+        <v>6.6E-3</v>
+      </c>
+      <c r="L28">
+        <v>0.1114</v>
+      </c>
+      <c r="M28">
+        <v>0.10086000000000001</v>
+      </c>
+      <c r="N28">
+        <v>0.12195</v>
+      </c>
+      <c r="O28">
+        <v>5.3800000000000002E-3</v>
+      </c>
+      <c r="P28" s="1">
+        <v>7.9477199999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>2016</v>
+      </c>
+      <c r="C29">
+        <v>2016</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>228</v>
+      </c>
+      <c r="G29">
+        <v>164048590</v>
+      </c>
+      <c r="H29">
+        <v>0.13897999999999999</v>
+      </c>
+      <c r="I29">
+        <v>0.12094000000000001</v>
+      </c>
+      <c r="J29">
+        <v>0.15701999999999999</v>
+      </c>
+      <c r="K29">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="L29">
+        <v>0.1048</v>
+      </c>
+      <c r="M29">
+        <v>9.1079999999999994E-2</v>
+      </c>
+      <c r="N29">
+        <v>0.11852</v>
+      </c>
+      <c r="O29">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="P29" s="1">
+        <v>4.0268499999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>2016</v>
+      </c>
+      <c r="C30">
+        <v>2016</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30">
+        <v>231</v>
+      </c>
+      <c r="G30">
+        <v>159078923</v>
+      </c>
+      <c r="H30">
+        <v>0.14521000000000001</v>
+      </c>
+      <c r="I30">
+        <v>0.12648000000000001</v>
+      </c>
+      <c r="J30">
+        <v>0.16394</v>
+      </c>
+      <c r="K30">
+        <v>9.5499999999999995E-3</v>
+      </c>
+      <c r="L30">
+        <v>0.12772</v>
+      </c>
+      <c r="M30">
+        <v>0.11076</v>
+      </c>
+      <c r="N30">
+        <v>0.14466999999999999</v>
+      </c>
+      <c r="O30">
+        <v>8.6499999999999997E-3</v>
+      </c>
+      <c r="P30" s="1">
+        <v>4.0798300000000003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>2016</v>
+      </c>
+      <c r="C31">
+        <v>2016</v>
+      </c>
+      <c r="F31">
+        <v>459</v>
+      </c>
+      <c r="G31">
+        <v>323127513</v>
+      </c>
+      <c r="H31">
+        <v>0.14205000000000001</v>
+      </c>
+      <c r="I31">
+        <v>0.12905</v>
+      </c>
+      <c r="J31">
+        <v>0.15504000000000001</v>
+      </c>
+      <c r="K31">
+        <v>6.6299999999999996E-3</v>
+      </c>
+      <c r="L31">
+        <v>0.11296</v>
+      </c>
+      <c r="M31">
+        <v>0.10245</v>
+      </c>
+      <c r="N31">
+        <v>0.12347</v>
+      </c>
+      <c r="O31">
+        <v>5.3600000000000002E-3</v>
+      </c>
+      <c r="P31" s="1">
+        <v>8.1066799999999994E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>2017</v>
+      </c>
+      <c r="C32">
+        <v>2017</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>242</v>
+      </c>
+      <c r="G32">
+        <v>165311059</v>
+      </c>
+      <c r="H32">
+        <v>0.14638999999999999</v>
+      </c>
+      <c r="I32">
+        <v>0.12795000000000001</v>
+      </c>
+      <c r="J32">
+        <v>0.16483</v>
+      </c>
+      <c r="K32">
+        <v>9.41E-3</v>
+      </c>
+      <c r="L32">
+        <v>0.10773000000000001</v>
+      </c>
+      <c r="M32">
+        <v>9.3670000000000003E-2</v>
+      </c>
+      <c r="N32">
+        <v>0.12180000000000001</v>
+      </c>
+      <c r="O32">
+        <v>7.1799999999999998E-3</v>
+      </c>
+      <c r="P32" s="1">
+        <v>4.2741099999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>2017</v>
+      </c>
+      <c r="C33">
+        <v>2017</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>216</v>
+      </c>
+      <c r="G33">
+        <v>160408119</v>
+      </c>
+      <c r="H33">
+        <v>0.13466</v>
+      </c>
+      <c r="I33">
+        <v>0.1167</v>
+      </c>
+      <c r="J33">
+        <v>0.15261</v>
+      </c>
+      <c r="K33">
+        <v>9.1599999999999997E-3</v>
+      </c>
+      <c r="L33">
+        <v>0.11817999999999999</v>
+      </c>
+      <c r="M33">
+        <v>0.10181999999999999</v>
+      </c>
+      <c r="N33">
+        <v>0.13453999999999999</v>
+      </c>
+      <c r="O33">
+        <v>8.3499999999999998E-3</v>
+      </c>
+      <c r="P33" s="1">
+        <v>3.8149099999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>2017</v>
+      </c>
+      <c r="C34">
+        <v>2017</v>
+      </c>
+      <c r="F34">
+        <v>458</v>
+      </c>
+      <c r="G34">
+        <v>325719178</v>
+      </c>
+      <c r="H34">
+        <v>0.14061000000000001</v>
+      </c>
+      <c r="I34">
+        <v>0.12773000000000001</v>
+      </c>
+      <c r="J34">
+        <v>0.15348999999999999</v>
+      </c>
+      <c r="K34">
+        <v>6.5700000000000003E-3</v>
+      </c>
+      <c r="L34">
+        <v>0.10635</v>
+      </c>
+      <c r="M34">
+        <v>9.6240000000000006E-2</v>
+      </c>
+      <c r="N34">
+        <v>0.11645999999999999</v>
+      </c>
+      <c r="O34">
+        <v>5.1599999999999997E-3</v>
+      </c>
+      <c r="P34" s="1">
+        <v>8.0890100000000006E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>2018</v>
+      </c>
+      <c r="C35">
+        <v>2018</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35">
+        <v>227</v>
+      </c>
+      <c r="G35">
+        <v>166038755</v>
+      </c>
+      <c r="H35">
+        <v>0.13672000000000001</v>
+      </c>
+      <c r="I35">
+        <v>0.11892999999999999</v>
+      </c>
+      <c r="J35">
+        <v>0.1545</v>
+      </c>
+      <c r="K35">
+        <v>9.0699999999999999E-3</v>
+      </c>
+      <c r="L35">
+        <v>9.8199999999999996E-2</v>
+      </c>
+      <c r="M35">
+        <v>8.4919999999999995E-2</v>
+      </c>
+      <c r="N35">
+        <v>0.11147</v>
+      </c>
+      <c r="O35">
+        <v>6.77E-3</v>
+      </c>
+      <c r="P35" s="1">
+        <v>4.0091799999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>2018</v>
+      </c>
+      <c r="C36">
+        <v>2018</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36">
+        <v>213</v>
+      </c>
+      <c r="G36">
+        <v>161128679</v>
+      </c>
+      <c r="H36">
+        <v>0.13219</v>
+      </c>
+      <c r="I36">
+        <v>0.11444</v>
+      </c>
+      <c r="J36">
+        <v>0.14995</v>
+      </c>
+      <c r="K36">
+        <v>9.0600000000000003E-3</v>
+      </c>
+      <c r="L36">
+        <v>0.11296</v>
+      </c>
+      <c r="M36">
+        <v>9.6949999999999995E-2</v>
+      </c>
+      <c r="N36">
+        <v>0.12897</v>
+      </c>
+      <c r="O36">
+        <v>8.1700000000000002E-3</v>
+      </c>
+      <c r="P36" s="1">
+        <v>3.7619199999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>2018</v>
+      </c>
+      <c r="C37">
+        <v>2018</v>
+      </c>
+      <c r="F37">
+        <v>440</v>
+      </c>
+      <c r="G37">
+        <v>327167434</v>
+      </c>
+      <c r="H37">
+        <v>0.13449</v>
+      </c>
+      <c r="I37">
+        <v>0.12192</v>
+      </c>
+      <c r="J37">
+        <v>0.14704999999999999</v>
+      </c>
+      <c r="K37">
+        <v>6.4099999999999999E-3</v>
+      </c>
+      <c r="L37">
+        <v>0.1048</v>
+      </c>
+      <c r="M37">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="N37">
+        <v>0.115</v>
+      </c>
+      <c r="O37">
+        <v>5.2100000000000002E-3</v>
+      </c>
+      <c r="P37" s="1">
+        <v>7.7711100000000005E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>2019</v>
+      </c>
+      <c r="C38">
+        <v>2019</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38">
         <v>259</v>
       </c>
-      <c r="G27">
+      <c r="G38">
+        <v>166582199</v>
+      </c>
+      <c r="H38">
+        <v>0.15548000000000001</v>
+      </c>
+      <c r="I38">
+        <v>0.13653999999999999</v>
+      </c>
+      <c r="J38">
+        <v>0.17441000000000001</v>
+      </c>
+      <c r="K38">
+        <v>9.6600000000000002E-3</v>
+      </c>
+      <c r="L38">
+        <v>0.10985</v>
+      </c>
+      <c r="M38">
+        <v>9.6259999999999998E-2</v>
+      </c>
+      <c r="N38">
+        <v>0.12345</v>
+      </c>
+      <c r="O38">
+        <v>6.9300000000000004E-3</v>
+      </c>
+      <c r="P38" s="1">
+        <v>4.5743600000000002E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>2019</v>
+      </c>
+      <c r="C39">
+        <v>2019</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39">
+        <v>259</v>
+      </c>
+      <c r="G39">
         <v>161657324</v>
       </c>
-      <c r="H27">
+      <c r="H39">
         <v>0.16022</v>
       </c>
-      <c r="I27">
+      <c r="I39">
         <v>0.14069999999999999</v>
       </c>
-      <c r="J27">
+      <c r="J39">
         <v>0.17973</v>
       </c>
-      <c r="K27">
+      <c r="K39">
         <v>9.9600000000000001E-3</v>
       </c>
-      <c r="L27">
+      <c r="L39">
         <v>0.12404</v>
       </c>
-      <c r="M27">
+      <c r="M39">
         <v>0.10835</v>
       </c>
-      <c r="N27">
+      <c r="N39">
         <v>0.13974</v>
       </c>
-      <c r="O27">
+      <c r="O39">
         <v>8.0099999999999998E-3</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P39" s="1">
         <v>4.5743600000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B28">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>2019</v>
+      </c>
+      <c r="C40">
+        <v>2019</v>
+      </c>
+      <c r="F40">
+        <v>518</v>
+      </c>
+      <c r="G40">
+        <v>328239523</v>
+      </c>
+      <c r="H40">
+        <v>0.15781000000000001</v>
+      </c>
+      <c r="I40">
+        <v>0.14421999999999999</v>
+      </c>
+      <c r="J40">
+        <v>0.1714</v>
+      </c>
+      <c r="K40">
+        <v>6.9300000000000004E-3</v>
+      </c>
+      <c r="L40">
+        <v>0.11434</v>
+      </c>
+      <c r="M40">
+        <v>0.10417999999999999</v>
+      </c>
+      <c r="N40">
+        <v>0.1245</v>
+      </c>
+      <c r="O40">
+        <v>5.1799999999999997E-3</v>
+      </c>
+      <c r="P40" s="1">
+        <v>9.1487100000000002E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B41">
         <v>2020</v>
       </c>
-      <c r="C28">
+      <c r="C41">
         <v>2020</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D41" t="s">
         <v>16</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E41" t="s">
         <v>17</v>
       </c>
-      <c r="F28">
+      <c r="F41">
         <v>250</v>
       </c>
-      <c r="G28">
+      <c r="G41">
         <v>167227921</v>
       </c>
-      <c r="H28">
+      <c r="H41">
         <v>0.14949999999999999</v>
       </c>
-      <c r="I28">
+      <c r="I41">
         <v>0.13095999999999999</v>
       </c>
-      <c r="J28">
+      <c r="J41">
         <v>0.16803000000000001</v>
       </c>
-      <c r="K28">
+      <c r="K41">
         <v>9.4500000000000001E-3</v>
       </c>
-      <c r="L28">
+      <c r="L41">
         <v>0.11198</v>
       </c>
-      <c r="M28">
+      <c r="M41">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="N28">
+      <c r="N41">
         <v>0.12645000000000001</v>
       </c>
-      <c r="O28">
+      <c r="O41">
         <v>7.3800000000000003E-3</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P41" s="1">
         <v>4.4153999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B29">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B42">
         <v>2020</v>
       </c>
-      <c r="C29">
+      <c r="C42">
         <v>2020</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E42" t="s">
         <v>19</v>
       </c>
-      <c r="F29">
+      <c r="F42">
         <v>226</v>
       </c>
-      <c r="G29">
+      <c r="G42">
         <v>162256202</v>
       </c>
-      <c r="H29">
+      <c r="H42">
         <v>0.13929</v>
       </c>
-      <c r="I29">
+      <c r="I42">
         <v>0.12113</v>
       </c>
-      <c r="J29">
+      <c r="J42">
         <v>0.15745000000000001</v>
       </c>
-      <c r="K29">
+      <c r="K42">
         <v>9.2700000000000005E-3</v>
       </c>
-      <c r="L29">
+      <c r="L42">
         <v>0.11067</v>
       </c>
-      <c r="M29">
+      <c r="M42">
         <v>9.5610000000000001E-2</v>
       </c>
-      <c r="N29">
+      <c r="N42">
         <v>0.12573000000000001</v>
       </c>
-      <c r="O29">
+      <c r="O42">
         <v>7.6800000000000002E-3</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P42" s="1">
         <v>3.9915199999999998E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>2020</v>
+      </c>
+      <c r="C43">
+        <v>2020</v>
+      </c>
+      <c r="F43">
+        <v>476</v>
+      </c>
+      <c r="G43">
+        <v>329484123</v>
+      </c>
+      <c r="H43">
+        <v>0.14446999999999999</v>
+      </c>
+      <c r="I43">
+        <v>0.13149</v>
+      </c>
+      <c r="J43">
+        <v>0.15745000000000001</v>
+      </c>
+      <c r="K43">
+        <v>6.62E-3</v>
+      </c>
+      <c r="L43">
+        <v>0.11645999999999999</v>
+      </c>
+      <c r="M43">
+        <v>0.10564</v>
+      </c>
+      <c r="N43">
+        <v>0.12728</v>
+      </c>
+      <c r="O43">
+        <v>5.5199999999999997E-3</v>
+      </c>
+      <c r="P43" s="1">
+        <v>8.4069199999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <v>5662</v>
+      </c>
+      <c r="G44">
+        <v>4436490683</v>
+      </c>
+      <c r="H44">
+        <v>0.12762000000000001</v>
+      </c>
+      <c r="I44">
+        <v>0.12429999999999999</v>
+      </c>
+      <c r="J44">
+        <v>0.13095000000000001</v>
+      </c>
+      <c r="K44">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="L44">
+        <v>0.1048</v>
+      </c>
+      <c r="M44">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="N44">
+        <v>0.1076</v>
+      </c>
+      <c r="O44">
+        <v>1.4300000000000001E-3</v>
+      </c>
+      <c r="P44" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2534,353 +3191,353 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="111.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="111.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>